<commit_message>
Completed Excel Decimal Data Validation
</commit_message>
<xml_diff>
--- a/16 - Excel Data Validation/Excel102Exercises.xlsx
+++ b/16 - Excel Data Validation/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/16 - Excel Data Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AA948CF-7208-4A4E-A310-886A008857FC}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{345A9EBC-AC98-4499-A6B9-02A0DDE57754}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49789,7 +49789,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -50309,12 +50309,19 @@
       <c r="B20" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="I20" s="12">
+        <v>39.950000000000003</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B30" xr:uid="{484ECE3D-DD57-4E91-A8AD-BBE4D4E124A4}">
       <formula1>"Ford,Chevy,Pontiac,Oldsmobile,Dodge"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I30" xr:uid="{E0BBEE50-FB9A-490C-913F-083891303F85}">
+      <formula1>14.95</formula1>
+      <formula2>39.95</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Adding a Custom Excel Data Validation Error
</commit_message>
<xml_diff>
--- a/16 - Excel Data Validation/Excel102Exercises.xlsx
+++ b/16 - Excel Data Validation/Excel102Exercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/16 - Excel Data Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{345A9EBC-AC98-4499-A6B9-02A0DDE57754}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC457669-064F-4A37-980D-FCF17AD51C04}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49788,8 +49788,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -50316,7 +50316,7 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B30" xr:uid="{484ECE3D-DD57-4E91-A8AD-BBE4D4E124A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Car Make" error="You must pick a value from the drop down menu." sqref="B4:B30" xr:uid="{484ECE3D-DD57-4E91-A8AD-BBE4D4E124A4}">
       <formula1>"Ford,Chevy,Pontiac,Oldsmobile,Dodge"</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I30" xr:uid="{E0BBEE50-FB9A-490C-913F-083891303F85}">

</xml_diff>

<commit_message>
Completed Dynamic Formulas by Using Excel Data Validation Techniques
</commit_message>
<xml_diff>
--- a/16 - Excel Data Validation/Excel102Exercises.xlsx
+++ b/16 - Excel Data Validation/Excel102Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/16 - Excel Data Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC457669-064F-4A37-980D-FCF17AD51C04}"/>
+  <xr:revisionPtr revIDLastSave="254" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1ED4E3E-9C70-4546-B7E1-8F1A2C144AFF}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5056" uniqueCount="1438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5062" uniqueCount="1438">
   <si>
     <t>Town</t>
   </si>
@@ -8777,10 +8777,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8794,9 +8794,10 @@
     <col min="8" max="9" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="72" t="s">
         <v>119</v>
       </c>
@@ -8816,7 +8817,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>116</v>
       </c>
@@ -8848,8 +8849,11 @@
       <c r="K2" s="78" t="s">
         <v>1434</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>116</v>
       </c>
@@ -8883,8 +8887,11 @@
         <f>DAVERAGE(A1:F59,F1,H2:I4)</f>
         <v>10932.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>116</v>
       </c>
@@ -8910,8 +8917,11 @@
       <c r="I4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>116</v>
       </c>
@@ -8931,8 +8941,11 @@
         <f t="shared" si="0"/>
         <v>3750</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>116</v>
       </c>
@@ -8952,8 +8965,11 @@
         <f t="shared" si="0"/>
         <v>5875</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>116</v>
       </c>
@@ -8982,8 +8998,11 @@
       <c r="J7" s="78" t="s">
         <v>1435</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="N7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>116</v>
       </c>
@@ -9012,7 +9031,7 @@
       </c>
       <c r="K8" s="79"/>
     </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>116</v>
       </c>
@@ -9033,7 +9052,7 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>116</v>
       </c>
@@ -9054,7 +9073,7 @@
         <v>24465</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>116</v>
       </c>
@@ -9081,7 +9100,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>116</v>
       </c>
@@ -9110,7 +9129,7 @@
         <v>1428320</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>116</v>
       </c>
@@ -9131,7 +9150,7 @@
         <v>36500</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
         <v>116</v>
       </c>
@@ -9152,7 +9171,7 @@
         <v>37250</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
         <v>116</v>
       </c>
@@ -9173,7 +9192,7 @@
         <v>75390</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
         <v>115</v>
       </c>
@@ -10099,6 +10118,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I5" xr:uid="{CD1F4B09-308F-4591-89F2-03CBCF665FA0}">
+      <formula1>$N$2:$N$7</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions gridLinesSet="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -49788,7 +49812,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>